<commit_message>
ok now finished maybe
</commit_message>
<xml_diff>
--- a/app/generic_sheet/generic_sheet.xlsx
+++ b/app/generic_sheet/generic_sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="1100" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="37">
   <si>
     <t>Monday</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Fall schedule goes on top, winter schedule goes underneath that, summer schedule goes on the bottom</t>
+  </si>
+  <si>
+    <t>9:00-9:30 PM</t>
+  </si>
+  <si>
+    <t>9:30-10:00 PM</t>
   </si>
 </sst>
 </file>
@@ -172,8 +178,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -200,7 +214,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -212,6 +226,10 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -223,6 +241,10 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -552,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -715,295 +737,324 @@
         <v>28</v>
       </c>
     </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="27" spans="1:8">
-      <c r="B27" t="s">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="B29" t="s">
         <v>0</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>1</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D29" t="s">
         <v>2</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E29" t="s">
         <v>3</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F29" t="s">
         <v>4</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G29" t="s">
         <v>32</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H29" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="B53" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" t="s">
-        <v>1</v>
-      </c>
-      <c r="D53" t="s">
-        <v>2</v>
-      </c>
-      <c r="E53" t="s">
-        <v>3</v>
-      </c>
-      <c r="F53" t="s">
-        <v>4</v>
-      </c>
-      <c r="G53" t="s">
-        <v>32</v>
-      </c>
-      <c r="H53" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" t="s">
-        <v>8</v>
+      <c r="B57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" t="s">
+        <v>3</v>
+      </c>
+      <c r="F57" t="s">
+        <v>4</v>
+      </c>
+      <c r="G57" t="s">
+        <v>32</v>
+      </c>
+      <c r="H57" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>